<commit_message>
new changes to script
</commit_message>
<xml_diff>
--- a/synuclein_inclusion_biogenesis_2024/image_analysis/linoleic_acid/061725_SUMMARY.xlsx
+++ b/synuclein_inclusion_biogenesis_2024/image_analysis/linoleic_acid/061725_SUMMARY.xlsx
@@ -760,10 +760,10 @@
         <v>150.5</v>
       </c>
       <c r="H7" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I7" t="n">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
         <v>3</v>
@@ -1542,10 +1542,10 @@
         <v>105.3333333333333</v>
       </c>
       <c r="H24" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I24" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="n">
         <v>3</v>
@@ -1864,10 +1864,10 @@
         <v>415.1666666666667</v>
       </c>
       <c r="H31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I31" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
         <v>4</v>
@@ -2094,10 +2094,10 @@
         <v>289.6666666666667</v>
       </c>
       <c r="H36" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I36" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J36" t="n">
         <v>3</v>
@@ -2186,10 +2186,10 @@
         <v>485.625</v>
       </c>
       <c r="H38" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I38" t="n">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="J38" t="n">
         <v>4</v>
@@ -2278,10 +2278,10 @@
         <v>294.7142857142857</v>
       </c>
       <c r="H40" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I40" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="J40" t="n">
         <v>7</v>
@@ -2508,10 +2508,10 @@
         <v>559</v>
       </c>
       <c r="H45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I45" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J45" t="n">
         <v>1</v>
@@ -2784,10 +2784,10 @@
         <v>1411.5</v>
       </c>
       <c r="H51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I51" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J51" t="n">
         <v>1</v>
@@ -3290,10 +3290,10 @@
         <v>677.75</v>
       </c>
       <c r="H62" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I62" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J62" t="n">
         <v>5</v>
@@ -3382,10 +3382,10 @@
         <v>1719.333333333333</v>
       </c>
       <c r="H64" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I64" t="n">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="J64" t="n">
         <v>3</v>
@@ -3520,10 +3520,10 @@
         <v>351.6</v>
       </c>
       <c r="H67" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I67" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="J67" t="n">
         <v>2</v>
@@ -3658,10 +3658,10 @@
         <v>165.75</v>
       </c>
       <c r="H70" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I70" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J70" t="n">
         <v>3</v>
@@ -3888,10 +3888,10 @@
         <v>489</v>
       </c>
       <c r="H75" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I75" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="J75" t="n">
         <v>5</v>
@@ -4026,10 +4026,10 @@
         <v>938.5</v>
       </c>
       <c r="H78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J78" t="n">
         <v>2</v>
@@ -4118,10 +4118,10 @@
         <v>467.7142857142857</v>
       </c>
       <c r="H80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I80" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J80" t="n">
         <v>4</v>
@@ -4210,10 +4210,10 @@
         <v>2337</v>
       </c>
       <c r="H82" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I82" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J82" t="n">
         <v>2</v>
@@ -4256,10 +4256,10 @@
         <v>366.3</v>
       </c>
       <c r="H83" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I83" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J83" t="n">
         <v>5</v>
@@ -4394,10 +4394,10 @@
         <v>331.75</v>
       </c>
       <c r="H86" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I86" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J86" t="n">
         <v>3</v>
@@ -4624,10 +4624,10 @@
         <v>246</v>
       </c>
       <c r="H91" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J91" t="n">
         <v>2</v>
@@ -4762,10 +4762,10 @@
         <v>362.75</v>
       </c>
       <c r="H94" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I94" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J94" t="n">
         <v>7</v>
@@ -4854,10 +4854,10 @@
         <v>151</v>
       </c>
       <c r="H96" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I96" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J96" t="n">
         <v>2</v>
@@ -4900,10 +4900,10 @@
         <v>522.5</v>
       </c>
       <c r="H97" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I97" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="J97" t="n">
         <v>3</v>
@@ -4946,10 +4946,10 @@
         <v>146.8571428571429</v>
       </c>
       <c r="H98" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I98" t="n">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="J98" t="n">
         <v>2</v>
@@ -5314,10 +5314,10 @@
         <v>365.25</v>
       </c>
       <c r="H106" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I106" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J106" t="n">
         <v>1</v>
@@ -6326,10 +6326,10 @@
         <v>80.83333333333333</v>
       </c>
       <c r="H128" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I128" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J128" t="n">
         <v>3</v>
@@ -6418,10 +6418,10 @@
         <v>65.75</v>
       </c>
       <c r="H130" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I130" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J130" t="n">
         <v>1</v>
@@ -6832,10 +6832,10 @@
         <v>189.4</v>
       </c>
       <c r="H139" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I139" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J139" t="n">
         <v>1</v>
@@ -8396,10 +8396,10 @@
         <v>206.1111111111111</v>
       </c>
       <c r="H173" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I173" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J173" t="n">
         <v>3</v>
@@ -8534,10 +8534,10 @@
         <v>164</v>
       </c>
       <c r="H176" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I176" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J176" t="n">
         <v>6</v>
@@ -8764,10 +8764,10 @@
         <v>1397</v>
       </c>
       <c r="H181" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I181" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J181" t="n">
         <v>2</v>
@@ -8902,10 +8902,10 @@
         <v>188.25</v>
       </c>
       <c r="H184" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I184" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J184" t="n">
         <v>3</v>
@@ -9040,10 +9040,10 @@
         <v>3493</v>
       </c>
       <c r="H187" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I187" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J187" t="n">
         <v>3</v>
@@ -11156,10 +11156,10 @@
         <v>235.9</v>
       </c>
       <c r="H233" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I233" t="n">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="J233" t="n">
         <v>6</v>
@@ -12996,10 +12996,10 @@
         <v>178.5</v>
       </c>
       <c r="H273" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I273" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J273" t="n">
         <v>4</v>
@@ -13088,10 +13088,10 @@
         <v>446.8571428571428</v>
       </c>
       <c r="H275" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I275" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J275" t="n">
         <v>3</v>
@@ -13778,10 +13778,10 @@
         <v>76.75</v>
       </c>
       <c r="H290" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I290" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J290" t="n">
         <v>1</v>
@@ -14514,10 +14514,10 @@
         <v>201</v>
       </c>
       <c r="H306" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I306" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J306" t="n">
         <v>4</v>
@@ -15020,10 +15020,10 @@
         <v>259.3333333333333</v>
       </c>
       <c r="H317" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I317" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J317" t="n">
         <v>3</v>
@@ -16400,10 +16400,10 @@
         <v>239.375</v>
       </c>
       <c r="H347" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I347" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="J347" t="n">
         <v>4</v>
@@ -18378,10 +18378,10 @@
         <v>986.75</v>
       </c>
       <c r="H390" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="I390" t="n">
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="J390" t="n">
         <v>13</v>
@@ -19206,10 +19206,10 @@
         <v>243.4444444444445</v>
       </c>
       <c r="H408" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I408" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="J408" t="n">
         <v>2</v>
@@ -19482,10 +19482,10 @@
         <v>37.75</v>
       </c>
       <c r="H414" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I414" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J414" t="n">
         <v>4</v>
@@ -22104,10 +22104,10 @@
         <v>153.9090909090909</v>
       </c>
       <c r="H471" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I471" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J471" t="n">
         <v>6</v>
@@ -23438,10 +23438,10 @@
         <v>42.25</v>
       </c>
       <c r="H500" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I500" t="n">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="J500" t="n">
         <v>2</v>
@@ -25232,10 +25232,10 @@
         <v>527.75</v>
       </c>
       <c r="H539" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I539" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J539" t="n">
         <v>8</v>
@@ -25370,10 +25370,10 @@
         <v>19</v>
       </c>
       <c r="H542" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I542" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J542" t="n">
         <v>1</v>
@@ -25554,10 +25554,10 @@
         <v>384</v>
       </c>
       <c r="H546" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I546" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J546" t="n">
         <v>2</v>
@@ -25646,10 +25646,10 @@
         <v>921.3333333333334</v>
       </c>
       <c r="H548" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I548" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J548" t="n">
         <v>3</v>
@@ -25784,10 +25784,10 @@
         <v>1484</v>
       </c>
       <c r="H551" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I551" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J551" t="n">
         <v>2</v>
@@ -26152,10 +26152,10 @@
         <v>701.4</v>
       </c>
       <c r="H559" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I559" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J559" t="n">
         <v>4</v>
@@ -26704,10 +26704,10 @@
         <v>120.6666666666667</v>
       </c>
       <c r="H571" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I571" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J571" t="n">
         <v>4</v>
@@ -26796,10 +26796,10 @@
         <v>905.3333333333334</v>
       </c>
       <c r="H573" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I573" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J573" t="n">
         <v>6</v>
@@ -27808,10 +27808,10 @@
         <v>1149</v>
       </c>
       <c r="H595" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I595" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J595" t="n">
         <v>1</v>
@@ -28084,10 +28084,10 @@
         <v>231</v>
       </c>
       <c r="H601" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I601" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J601" t="n">
         <v>6</v>
@@ -28222,10 +28222,10 @@
         <v>451.3333333333333</v>
       </c>
       <c r="H604" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I604" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J604" t="n">
         <v>3</v>
@@ -28590,10 +28590,10 @@
         <v>715.5</v>
       </c>
       <c r="H612" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I612" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J612" t="n">
         <v>1</v>
@@ -29096,10 +29096,10 @@
         <v>310.1666666666667</v>
       </c>
       <c r="H623" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I623" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J623" t="n">
         <v>5</v>
@@ -30338,10 +30338,10 @@
         <v>343.3636363636364</v>
       </c>
       <c r="H650" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I650" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J650" t="n">
         <v>4</v>
@@ -30522,10 +30522,10 @@
         <v>463.8</v>
       </c>
       <c r="H654" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I654" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J654" t="n">
         <v>1</v>
@@ -31028,10 +31028,10 @@
         <v>179.7692307692308</v>
       </c>
       <c r="H665" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I665" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J665" t="n">
         <v>7</v>
@@ -31856,10 +31856,10 @@
         <v>62</v>
       </c>
       <c r="H683" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I683" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J683" t="n">
         <v>4</v>
@@ -33512,10 +33512,10 @@
         <v>199.4615384615385</v>
       </c>
       <c r="H719" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I719" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J719" t="n">
         <v>6</v>
@@ -34156,10 +34156,10 @@
         <v>327.3636363636364</v>
       </c>
       <c r="H733" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I733" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J733" t="n">
         <v>4</v>
@@ -36318,10 +36318,10 @@
         <v>95</v>
       </c>
       <c r="H780" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I780" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J780" t="n">
         <v>3</v>
@@ -38158,10 +38158,10 @@
         <v>214.375</v>
       </c>
       <c r="H820" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I820" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J820" t="n">
         <v>5</v>
@@ -39216,10 +39216,10 @@
         <v>77.5</v>
       </c>
       <c r="H843" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I843" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J843" t="n">
         <v>1</v>
@@ -39446,10 +39446,10 @@
         <v>50</v>
       </c>
       <c r="H848" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I848" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J848" t="n">
         <v>3</v>
@@ -40918,10 +40918,10 @@
         <v>536</v>
       </c>
       <c r="H880" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I880" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="J880" t="n">
         <v>2</v>
@@ -41470,10 +41470,10 @@
         <v>76.57142857142857</v>
       </c>
       <c r="H892" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I892" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J892" t="n">
         <v>5</v>
@@ -41608,10 +41608,10 @@
         <v>80.5</v>
       </c>
       <c r="H895" t="n">
+        <v>5</v>
+      </c>
+      <c r="I895" t="n">
         <v>6</v>
-      </c>
-      <c r="I895" t="n">
-        <v>5</v>
       </c>
       <c r="J895" t="n">
         <v>11</v>
@@ -42022,10 +42022,10 @@
         <v>263</v>
       </c>
       <c r="H904" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I904" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J904" t="n">
         <v>8</v>
@@ -43034,10 +43034,10 @@
         <v>79.5</v>
       </c>
       <c r="H926" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I926" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J926" t="n">
         <v>3</v>
@@ -43126,10 +43126,10 @@
         <v>66</v>
       </c>
       <c r="H928" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I928" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="J928" t="n">
         <v>2</v>
@@ -43402,10 +43402,10 @@
         <v>66.5</v>
       </c>
       <c r="H934" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I934" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J934" t="n">
         <v>2</v>
@@ -43908,10 +43908,10 @@
         <v>340.4</v>
       </c>
       <c r="H945" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I945" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J945" t="n">
         <v>3</v>
@@ -44138,10 +44138,10 @@
         <v>143.375</v>
       </c>
       <c r="H950" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I950" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J950" t="n">
         <v>8</v>
@@ -44276,10 +44276,10 @@
         <v>354.4285714285714</v>
       </c>
       <c r="H953" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I953" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J953" t="n">
         <v>2</v>
@@ -44368,10 +44368,10 @@
         <v>353.4166666666667</v>
       </c>
       <c r="H955" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I955" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J955" t="n">
         <v>3</v>
@@ -45380,10 +45380,10 @@
         <v>94.92857142857143</v>
       </c>
       <c r="H977" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I977" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J977" t="n">
         <v>4</v>
@@ -46530,10 +46530,10 @@
         <v>233.4615384615385</v>
       </c>
       <c r="H1002" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1002" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J1002" t="n">
         <v>1</v>
@@ -49152,10 +49152,10 @@
         <v>292.3</v>
       </c>
       <c r="H1059" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I1059" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="J1059" t="n">
         <v>1</v>
@@ -49980,10 +49980,10 @@
         <v>72.5</v>
       </c>
       <c r="H1077" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I1077" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J1077" t="n">
         <v>2</v>
@@ -50118,10 +50118,10 @@
         <v>222.2222222222222</v>
       </c>
       <c r="H1080" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I1080" t="n">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="J1080" t="n">
         <v>6</v>
@@ -50440,10 +50440,10 @@
         <v>208.6</v>
       </c>
       <c r="H1087" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I1087" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J1087" t="n">
         <v>6</v>
@@ -51038,10 +51038,10 @@
         <v>232.1111111111111</v>
       </c>
       <c r="H1100" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I1100" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="J1100" t="n">
         <v>5</v>
@@ -51452,10 +51452,10 @@
         <v>90.25</v>
       </c>
       <c r="H1109" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I1109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J1109" t="n">
         <v>3</v>
@@ -58628,10 +58628,10 @@
         <v>93</v>
       </c>
       <c r="H1265" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1265" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1265" t="n">
         <v>10</v>
@@ -60422,10 +60422,10 @@
         <v>278.2</v>
       </c>
       <c r="H1304" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1304" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J1304" t="n">
         <v>2</v>
@@ -61066,10 +61066,10 @@
         <v>121</v>
       </c>
       <c r="H1318" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I1318" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J1318" t="n">
         <v>3</v>
@@ -61664,10 +61664,10 @@
         <v>65.2</v>
       </c>
       <c r="H1331" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I1331" t="n">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="J1331" t="n">
         <v>4</v>
@@ -61940,10 +61940,10 @@
         <v>185</v>
       </c>
       <c r="H1337" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1337" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J1337" t="n">
         <v>1</v>
@@ -62124,10 +62124,10 @@
         <v>185.6</v>
       </c>
       <c r="H1341" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I1341" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J1341" t="n">
         <v>2</v>
@@ -63504,10 +63504,10 @@
         <v>121.5</v>
       </c>
       <c r="H1371" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I1371" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J1371" t="n">
         <v>5</v>
@@ -63596,10 +63596,10 @@
         <v>343.3333333333333</v>
       </c>
       <c r="H1373" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I1373" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J1373" t="n">
         <v>4</v>
@@ -64010,10 +64010,10 @@
         <v>246</v>
       </c>
       <c r="H1382" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I1382" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J1382" t="n">
         <v>8</v>
@@ -65298,10 +65298,10 @@
         <v>225.7142857142857</v>
       </c>
       <c r="H1410" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I1410" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="J1410" t="n">
         <v>1</v>
@@ -66494,10 +66494,10 @@
         <v>92.25</v>
       </c>
       <c r="H1436" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I1436" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J1436" t="n">
         <v>2</v>
@@ -66770,10 +66770,10 @@
         <v>111.6666666666667</v>
       </c>
       <c r="H1442" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I1442" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="J1442" t="n">
         <v>4</v>
@@ -67276,10 +67276,10 @@
         <v>91.5</v>
       </c>
       <c r="H1453" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1453" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J1453" t="n">
         <v>1</v>
@@ -67552,10 +67552,10 @@
         <v>202</v>
       </c>
       <c r="H1459" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1459" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J1459" t="n">
         <v>1</v>
@@ -67782,10 +67782,10 @@
         <v>423</v>
       </c>
       <c r="H1464" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I1464" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J1464" t="n">
         <v>2</v>
@@ -67920,10 +67920,10 @@
         <v>173.3333333333333</v>
       </c>
       <c r="H1467" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I1467" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="J1467" t="n">
         <v>9</v>
@@ -69668,10 +69668,10 @@
         <v>14.5</v>
       </c>
       <c r="H1505" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1505" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J1505" t="n">
         <v>2</v>
@@ -71554,10 +71554,10 @@
         <v>355</v>
       </c>
       <c r="H1546" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1546" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J1546" t="n">
         <v>1</v>
@@ -72198,10 +72198,10 @@
         <v>544</v>
       </c>
       <c r="H1560" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1560" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J1560" t="n">
         <v>3</v>
@@ -73440,10 +73440,10 @@
         <v>201.5</v>
       </c>
       <c r="H1587" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1587" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J1587" t="n">
         <v>1</v>
@@ -74130,10 +74130,10 @@
         <v>712</v>
       </c>
       <c r="H1602" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I1602" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J1602" t="n">
         <v>4</v>
@@ -74314,10 +74314,10 @@
         <v>475</v>
       </c>
       <c r="H1606" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I1606" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J1606" t="n">
         <v>4</v>
@@ -75004,10 +75004,10 @@
         <v>93.88888888888889</v>
       </c>
       <c r="H1621" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I1621" t="n">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J1621" t="n">
         <v>2</v>
@@ -77028,10 +77028,10 @@
         <v>92.92307692307692</v>
       </c>
       <c r="H1665" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I1665" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J1665" t="n">
         <v>6</v>
@@ -79052,10 +79052,10 @@
         <v>247.6666666666667</v>
       </c>
       <c r="H1709" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I1709" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J1709" t="n">
         <v>2</v>
@@ -79696,10 +79696,10 @@
         <v>106.2592592592593</v>
       </c>
       <c r="H1723" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I1723" t="n">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="J1723" t="n">
         <v>4</v>
@@ -80524,10 +80524,10 @@
         <v>45.66666666666666</v>
       </c>
       <c r="H1741" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1741" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J1741" t="n">
         <v>2</v>

</xml_diff>